<commit_message>
updated crosswalk- see CHANGELOG for details
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WUZ\Desktop\DSU\Salmon-SMU-CU-DU-Lookup-Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WUZ\Desktop\DSU\Salmon-SMU-CU-DU-Lookup-Table - Pacific_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5D28FD-57DD-4196-9A11-B05D21AB78FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74417F4C-AF58-4C8D-BB68-969526D9E6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="0" windowWidth="19125" windowHeight="10035" xr2:uid="{0AA31071-30F2-4C0C-B579-7B1123D31F09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0AA31071-30F2-4C0C-B579-7B1123D31F09}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="2" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>The CU was deleted after confirmation that no persistent populations were ever present within recorded history within the area of the CU. This category is used to manage changes to CUs, and is not a CU.</t>
   </si>
   <si>
-    <t>Species</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -211,18 +208,12 @@
     <t>SMU Name</t>
   </si>
   <si>
-    <t>Full SMU Index</t>
-  </si>
-  <si>
     <t>The assigned name of the Conservation Unit (CU).</t>
   </si>
   <si>
     <t>CU Name</t>
   </si>
   <si>
-    <t>Full CU Index</t>
-  </si>
-  <si>
     <t>CU Type</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Designatable Unit (DU) number. Please be aware that there are duplicate DU numbers as each species has consecutive DU numbers.</t>
-  </si>
-  <si>
-    <t>Full DU Index</t>
   </si>
   <si>
     <t>DU Acronym</t>
@@ -261,6 +249,18 @@
 b) sites where transplanted fish are enumerated under the premise that DFO is recreating an extinct CU; and
 c) sites where transplanted fish are enumerated outside the ecotypical zone of the source population and no claim is made of recreating an extinct CU.
 Hatchery sites are often classified as a Bin.</t>
+  </si>
+  <si>
+    <t>Species Name</t>
+  </si>
+  <si>
+    <t>SMU Full Index</t>
+  </si>
+  <si>
+    <t>CU Full Index</t>
+  </si>
+  <si>
+    <t>DU Full Index</t>
   </si>
 </sst>
 </file>
@@ -487,6 +487,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -504,9 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,7 +826,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,10 +857,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>20</v>
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>18</v>
@@ -885,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>6</v>
@@ -899,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>9</v>
@@ -916,7 +916,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>37</v>
@@ -927,10 +927,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="12"/>
     </row>
@@ -939,7 +939,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>16</v>
@@ -963,264 +963,264 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>56</v>
+      <c r="B10" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="22"/>
+      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="22"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="22"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="22"/>
+        <v>63</v>
+      </c>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="22"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="22"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="23"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="22"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="23"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="22"/>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="22"/>
+      <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="22"/>
+      <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="22"/>
+      <c r="D36" s="23"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="24"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D39" s="18"/>
     </row>
     <row r="40" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D41" s="18"/>
     </row>
@@ -1231,5 +1231,8 @@
     <mergeCell ref="D10:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified - Non-Classifié&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new column: CU Common Name
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WUZ\Desktop\DSU\Salmon-SMU-CU-DU-Lookup-Table - Pacific_science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74417F4C-AF58-4C8D-BB68-969526D9E6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFC40CA-D23F-4DF6-8C93-4062CFB54884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0AA31071-30F2-4C0C-B579-7B1123D31F09}"/>
+    <workbookView xWindow="10005" yWindow="465" windowWidth="19005" windowHeight="14340" xr2:uid="{0AA31071-30F2-4C0C-B579-7B1123D31F09}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Column Letter</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>DU Full Index</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CU Common Name</t>
+  </si>
+  <si>
+    <t>An informal or commonly used name for the Conservation Unit (CU)</t>
   </si>
 </sst>
 </file>
@@ -822,11 +831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBC8D39-FEDB-4485-8B62-E5A31DD07D7C}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,301 +943,313 @@
       </c>
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="25" t="s">
+    <row r="11" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="9" t="s">
-        <v>38</v>
+      <c r="C13" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="26"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="26"/>
-      <c r="C15" s="16" t="s">
-        <v>39</v>
-      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="26"/>
-      <c r="C16" s="17" t="s">
-        <v>40</v>
+      <c r="C16" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="26"/>
-      <c r="C17" s="7"/>
+      <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="26"/>
-      <c r="C18" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="23"/>
     </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="26"/>
-      <c r="C19" s="2" t="s">
-        <v>63</v>
+      <c r="C19" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="26"/>
-      <c r="C21" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="23"/>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="26"/>
-      <c r="C22" s="10" t="s">
-        <v>36</v>
+      <c r="C22" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="23"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="26"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="23"/>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="26"/>
-      <c r="C25" s="2" t="s">
-        <v>35</v>
+      <c r="C25" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D25" s="23"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="26"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="23"/>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="26"/>
-      <c r="C28" s="2" t="s">
-        <v>28</v>
+      <c r="C28" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D28" s="23"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="26"/>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="26"/>
-      <c r="C30" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="23"/>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="26"/>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
+      <c r="C31" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="D31" s="23"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="26"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="26"/>
-      <c r="C33" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="23"/>
     </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="26"/>
-      <c r="C34" s="2" t="s">
-        <v>32</v>
+      <c r="C34" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="D34" s="23"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="26"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="26"/>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="23"/>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="15" t="s">
+      <c r="D37" s="23"/>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="24"/>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" s="18"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>56</v>
+      <c r="B39" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C42" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D42" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A10:A37"/>
-    <mergeCell ref="B10:B37"/>
-    <mergeCell ref="D10:D37"/>
+    <mergeCell ref="A11:A38"/>
+    <mergeCell ref="B11:B38"/>
+    <mergeCell ref="D11:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>